<commit_message>
updated framework and books
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah.houdroge\Documents\GitHub\carbomica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C819E1-6C7D-4A22-851E-EEBC5DAA4FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708F7830-A69F-4088-A07A-092EA126E28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>aga-khan_hosp_KE</t>
   </si>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726CDC55-F78F-4D4F-AD5B-9673D5DF0E3F}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -482,8 +482,32 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -493,8 +517,32 @@
       <c r="C2" s="1">
         <v>1.2326984530234453</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E2">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H2">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I2">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J2">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -504,8 +552,32 @@
       <c r="C3" s="1">
         <v>0.39479588511188046</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E3">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H3">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I3">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J3">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -515,8 +587,32 @@
       <c r="C4" s="1">
         <v>5.0532408204755628</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E4">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H4">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I4">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J4">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -526,8 +622,32 @@
       <c r="C5" s="1">
         <v>1.053208013898892</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E5">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H5">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I5">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J5">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -537,8 +657,32 @@
       <c r="C6" s="1">
         <v>6.8788518451239415</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E6">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H6">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I6">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J6">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -548,8 +692,32 @@
       <c r="C7" s="1">
         <v>7.06</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E7">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H7">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I7">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J7">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -559,8 +727,32 @@
       <c r="C8" s="1">
         <v>5.2778604985793498</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E8">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H8">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I8">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J8">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -569,6 +761,30 @@
       </c>
       <c r="C9" s="1">
         <v>1.1266750676982307</v>
+      </c>
+      <c r="D9">
+        <v>0.33792134495884429</v>
+      </c>
+      <c r="E9">
+        <v>0.67735511513227553</v>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9">
+        <v>0.12954974111110007</v>
+      </c>
+      <c r="H9">
+        <v>0.72609968404906466</v>
+      </c>
+      <c r="I9">
+        <v>0.22184458107556482</v>
+      </c>
+      <c r="J9">
+        <v>0.7685331628046782</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -580,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB34176A-2DBB-4E55-BED7-E81047A94992}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,36 +847,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <f ca="1">RAND()*10000</f>
-        <v>2447.7528064080989</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:I2" ca="1" si="0">RAND()*10000</f>
-        <v>9658.0760150432798</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4760.0627260916108</v>
+        <v>600</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2593.621271194676</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>9007.1606216288219</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2109.4928730565689</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3483.3941638737765</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1821.9259710538061</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -668,36 +876,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:I9" ca="1" si="1">RAND()*10000</f>
-        <v>9570.7978792704998</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3881.1596121116286</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9606.5894863752601</v>
+        <v>600</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4789.2866600554062</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6470.6643774321838</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4651.7011789959188</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5433.5207028626255</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8318.3569922804763</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -705,36 +905,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9311.8972449369085</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9424.9998398584521</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4053.6483470042926</v>
+        <v>600</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>7701.0276336865272</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6789.2330375681277</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5317.366681488219</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5243.7648856801325</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9568.1385716836448</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -742,36 +934,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4275.005458467399</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5379.6975693797867</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4427.6470785803403</v>
+        <v>600</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9740.5894192899614</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2212.7264508960975</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1039.0510598634216</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>7553.7612232929105</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9860.5483494752261</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -779,36 +963,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6134.5934973755011</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1693.4147151304157</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6875.1602024720305</v>
+        <v>600</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5366.9395241990551</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8438.8491358364445</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3228.6839845803461</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>591.82365747652341</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1144.0033081735046</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -816,35 +992,27 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6170.3416368942944</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>4023.5092935694638</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>3028.7590579781854</v>
+        <v>600</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>838.51401252665437</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>7867.338450647012</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1983.2454556056643</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8496.1577543293188</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>4901.3646667208413</v>
       </c>
     </row>
@@ -853,36 +1021,28 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>590.83307673801653</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>929.65864852222137</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8775.060178054624</v>
+        <v>600</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9102.4531802361489</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5472.8096640778122</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2359.5720925855135</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6719.3776572781617</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8524.4387372850288</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -890,36 +1050,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2707.0835047961018</v>
+        <v>6170.3416368941998</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1127.0508411488056</v>
+        <v>4023.5092935694001</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>428.63800863845671</v>
+        <v>600</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>1584.2095717910786</v>
+        <v>8380.5140125266007</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9584.3703899689135</v>
+        <v>7867.3384506470002</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>2205.9092215974752</v>
+        <v>1983.2454556056</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>6115.0503368839127</v>
+        <v>8496.1577543293006</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>8555.9659487961908</v>
+        <v>4901.3646667208413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generation of input_data.xlsx
</commit_message>
<xml_diff>
--- a/input_data.xlsx
+++ b/input_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah.houdroge\Documents\GitHub\carbomica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A25DFC-4F1D-4F12-BEE6-4E6AE8F6A8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ED54C2-88AB-48EC-A000-E1586F00EE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
-    <sheet name="unit_costs" sheetId="2" r:id="rId2"/>
+    <sheet name="costs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>aga-khan_hosp_KE</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>chitse_rhcc_ZW</t>
-  </si>
-  <si>
-    <t>facilities</t>
   </si>
   <si>
     <t>facilities_number</t>
@@ -127,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +133,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,15 +164,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -486,7 +509,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,42 +528,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -575,7 +595,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -610,7 +630,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -645,7 +665,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -680,7 +700,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -715,7 +735,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -750,7 +770,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -785,7 +805,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -829,7 +849,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,36 +866,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
@@ -904,7 +921,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -933,7 +950,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
@@ -962,7 +979,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -991,7 +1008,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
@@ -1020,7 +1037,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
@@ -1049,7 +1066,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
@@ -1078,7 +1095,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">

</xml_diff>